<commit_message>
Mensaje de lo que cambiaste
</commit_message>
<xml_diff>
--- a/Source/BBVA.xlsx
+++ b/Source/BBVA.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="84">
   <si>
     <t xml:space="preserve">Fecha valor</t>
   </si>
@@ -233,6 +233,45 @@
   </si>
   <si>
     <t xml:space="preserve">11/01/2026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23/01/2026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">673 GADIS LA PALLOZA     A CORUÑA     ES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18/01/2026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Macenda (-A Coruña  17:38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Coruña -R.Guísamo 12:25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22/01/2026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EL CORTE INGLES-DEPARTAM.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ropa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20/01/2026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21/01/2026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19/01/2026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Netflix.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17/01/2026</t>
   </si>
 </sst>
 </file>
@@ -536,8 +575,8 @@
   </sheetPr>
   <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I28" activeCellId="0" sqref="I28"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I39" activeCellId="0" sqref="I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.62890625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1597,6 +1636,473 @@
         <v>25</v>
       </c>
     </row>
+    <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E37" s="3" t="n">
+        <v>-62.55</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G37" s="3" t="n">
+        <v>1155.39</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I37" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E38" s="3" t="n">
+        <v>-2.45</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G38" s="3" t="n">
+        <v>1217.94</v>
+      </c>
+      <c r="H38" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I38" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E39" s="3" t="n">
+        <v>-2.05</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G39" s="3" t="n">
+        <v>1220.39</v>
+      </c>
+      <c r="H39" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I39" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E40" s="3" t="n">
+        <v>-44.94</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G40" s="3" t="n">
+        <v>1222.44</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I40" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E41" s="3" t="n">
+        <v>-0.9</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G41" s="3" t="n">
+        <v>1267.38</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I41" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E42" s="3" t="n">
+        <v>-0.98</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G42" s="3" t="n">
+        <v>1268.28</v>
+      </c>
+      <c r="H42" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I42" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E43" s="3" t="n">
+        <v>-28.35</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G43" s="3" t="n">
+        <v>1269.26</v>
+      </c>
+      <c r="H43" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I43" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E44" s="3" t="n">
+        <v>-2.18</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G44" s="3" t="n">
+        <v>1297.61</v>
+      </c>
+      <c r="H44" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I44" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E45" s="3" t="n">
+        <v>-10.99</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G45" s="3" t="n">
+        <v>1299.79</v>
+      </c>
+      <c r="H45" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I45" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E46" s="3" t="n">
+        <v>-13.99</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G46" s="3" t="n">
+        <v>1310.78</v>
+      </c>
+      <c r="H46" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I46" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E47" s="3" t="n">
+        <v>-0.69</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G47" s="3" t="n">
+        <v>1324.77</v>
+      </c>
+      <c r="H47" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I47" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E48" s="3" t="n">
+        <v>-0.98</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G48" s="3" t="n">
+        <v>1325.46</v>
+      </c>
+      <c r="H48" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I48" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E49" s="3" t="n">
+        <v>-2.59</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G49" s="3" t="n">
+        <v>1326.44</v>
+      </c>
+      <c r="H49" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I49" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E50" s="3" t="n">
+        <v>-2.54</v>
+      </c>
+      <c r="F50" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G50" s="3" t="n">
+        <v>1329.03</v>
+      </c>
+      <c r="H50" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I50" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E51" s="3" t="n">
+        <v>-21.74</v>
+      </c>
+      <c r="F51" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G51" s="3" t="n">
+        <v>1331.57</v>
+      </c>
+      <c r="H51" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I51" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E52" s="3" t="n">
+        <v>-10.73</v>
+      </c>
+      <c r="F52" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G52" s="3" t="n">
+        <v>1353.31</v>
+      </c>
+      <c r="H52" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I52" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>